<commit_message>
deleted extra lines in the script
</commit_message>
<xml_diff>
--- a/predictionValues/answers_pred.xlsx
+++ b/predictionValues/answers_pred.xlsx
@@ -371,1082 +371,1082 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B2">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B3">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B4">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B5">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>0.8560506741599387</v>
+        <v>0.7602848156868673</v>
       </c>
       <c r="B6">
-        <v>0.1439493258400613</v>
+        <v>0.2397151843131327</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>0.5498452523359121</v>
+        <v>0.6420799356935972</v>
       </c>
       <c r="B7">
-        <v>0.4501547476640879</v>
+        <v>0.3579200643064028</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B8">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B9">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>0.6590750771611322</v>
+        <v>0.5659720316352707</v>
       </c>
       <c r="B10">
-        <v>0.3409249228388678</v>
+        <v>0.4340279683647293</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B11">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B12">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B13">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B14">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B15">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B16">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>0.7972827667242358</v>
+        <v>0.835482401800504</v>
       </c>
       <c r="B17">
-        <v>0.2027172332757642</v>
+        <v>0.164517598199496</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B18">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>0.6420799356935972</v>
+        <v>0.5498452523359121</v>
       </c>
       <c r="B19">
-        <v>0.3579200643064028</v>
+        <v>0.4501547476640879</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B20">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B21">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>0.8800592975468227</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B22">
-        <v>0.1199407024531773</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>0.8372691647646621</v>
+        <v>0.7329069162497991</v>
       </c>
       <c r="B23">
-        <v>0.1627308352353379</v>
+        <v>0.2670930837502009</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B24">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B25">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B26">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>0.6402498944296792</v>
+        <v>0.6401618593643882</v>
       </c>
       <c r="B27">
-        <v>0.3597501055703208</v>
+        <v>0.3598381406356118</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B28">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B29">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B30">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B31">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B32">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B33">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B34">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B35">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>0.850880607636742</v>
+        <v>0.863300632083034</v>
       </c>
       <c r="B36">
-        <v>0.149119392363258</v>
+        <v>0.136699367916966</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>0.5837959485783136</v>
+        <v>0.6335946406798525</v>
       </c>
       <c r="B37">
-        <v>0.4162040514216864</v>
+        <v>0.3664053593201475</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B38">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>0.6537986360375384</v>
+        <v>0.6661742215619185</v>
       </c>
       <c r="B39">
-        <v>0.3462013639624616</v>
+        <v>0.3338257784380815</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>0.6661742215619185</v>
+        <v>0.6537986360375384</v>
       </c>
       <c r="B40">
-        <v>0.3338257784380815</v>
+        <v>0.3462013639624616</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B41">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>0.6467096640978485</v>
+        <v>0.5998153575678875</v>
       </c>
       <c r="B42">
-        <v>0.3532903359021515</v>
+        <v>0.4001846424321125</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>0.6420799356935972</v>
+        <v>0.5498452523359121</v>
       </c>
       <c r="B43">
-        <v>0.3579200643064028</v>
+        <v>0.4501547476640879</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>0.7589738888464646</v>
+        <v>0.7607555257210576</v>
       </c>
       <c r="B44">
-        <v>0.2410261111535354</v>
+        <v>0.2392444742789424</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>0.625729577345866</v>
+        <v>0.4829102216903616</v>
       </c>
       <c r="B45">
-        <v>0.374270422654134</v>
+        <v>0.5170897783096384</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>0.7242926823227368</v>
+        <v>0.801630212515808</v>
       </c>
       <c r="B46">
-        <v>0.2757073176772632</v>
+        <v>0.198369787484192</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>0.4096703063878999</v>
+        <v>0.5071022729512122</v>
       </c>
       <c r="B47">
-        <v>0.5903296936121001</v>
+        <v>0.4928977270487878</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B48">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B49">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B50">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B51">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B52">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B53">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B54">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B55">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>0.5732352212994309</v>
+        <v>0.4309734809161656</v>
       </c>
       <c r="B56">
-        <v>0.4267647787005691</v>
+        <v>0.5690265190838344</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B57">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>0.8753608052533827</v>
+        <v>0.8700720494148051</v>
       </c>
       <c r="B58">
-        <v>0.1246391947466173</v>
+        <v>0.1299279505851949</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B59">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>0.704513310412761</v>
+        <v>0.6612729355809915</v>
       </c>
       <c r="B60">
-        <v>0.295486689587239</v>
+        <v>0.3387270644190085</v>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B61">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B62">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B63">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>0.8700720494148051</v>
+        <v>0.8954638149707839</v>
       </c>
       <c r="B64">
-        <v>0.1299279505851949</v>
+        <v>0.1045361850292161</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B65">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B66">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>0.8954638149707839</v>
+        <v>0.8700720494148051</v>
       </c>
       <c r="B67">
-        <v>0.1045361850292161</v>
+        <v>0.1299279505851949</v>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>0.6467096640978485</v>
+        <v>0.5998153575678875</v>
       </c>
       <c r="B68">
-        <v>0.3532903359021515</v>
+        <v>0.4001846424321125</v>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>0.6618479884532266</v>
+        <v>0.5655337270146484</v>
       </c>
       <c r="B69">
-        <v>0.3381520115467734</v>
+        <v>0.4344662729853516</v>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B70">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B71">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B72">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>0.5998153575678875</v>
+        <v>0.6467096640978485</v>
       </c>
       <c r="B73">
-        <v>0.4001846424321125</v>
+        <v>0.3532903359021515</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B74">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>0.6388909624565985</v>
+        <v>0.5464150277543774</v>
       </c>
       <c r="B75">
-        <v>0.3611090375434015</v>
+        <v>0.4535849722456226</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B76">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B77">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>0.6995323775987874</v>
+        <v>0.6181347653176266</v>
       </c>
       <c r="B78">
-        <v>0.3004676224012126</v>
+        <v>0.3818652346823734</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B79">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>0.8982324901717611</v>
+        <v>0.873418168661053</v>
       </c>
       <c r="B80">
-        <v>0.1017675098282389</v>
+        <v>0.126581831338947</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B81">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B82">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B83">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B84">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B85">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B86">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="87">
       <c r="A87">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B87">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="88">
       <c r="A88">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B88">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="89">
       <c r="A89">
-        <v>0.8583034885215702</v>
+        <v>0.8856930230787471</v>
       </c>
       <c r="B89">
-        <v>0.1416965114784298</v>
+        <v>0.1143069769212529</v>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>0.7793707460362599</v>
+        <v>0.8101268523212063</v>
       </c>
       <c r="B90">
-        <v>0.2206292539637401</v>
+        <v>0.1898731476787937</v>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>0.7042392952545217</v>
+        <v>0.7441171837957787</v>
       </c>
       <c r="B91">
-        <v>0.2957607047454783</v>
+        <v>0.2558828162042213</v>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>0.697149626866256</v>
+        <v>0.8171955475183693</v>
       </c>
       <c r="B92">
-        <v>0.302850373133744</v>
+        <v>0.1828044524816307</v>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B93">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="94">
       <c r="A94">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B94">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="95">
       <c r="A95">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B95">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="96">
       <c r="A96">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B96">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="97">
       <c r="A97">
-        <v>0.8448363047213923</v>
+        <v>0.7797145041502886</v>
       </c>
       <c r="B97">
-        <v>0.1551636952786077</v>
+        <v>0.2202854958497114</v>
       </c>
     </row>
     <row r="98">
       <c r="A98">
-        <v>0.6852788780413201</v>
+        <v>0.6406594588827165</v>
       </c>
       <c r="B98">
-        <v>0.3147211219586799</v>
+        <v>0.3593405411172835</v>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>0.7242926823227368</v>
+        <v>0.801630212515808</v>
       </c>
       <c r="B99">
-        <v>0.2757073176772632</v>
+        <v>0.198369787484192</v>
       </c>
     </row>
     <row r="100">
       <c r="A100">
-        <v>0.8800592975468227</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B100">
-        <v>0.1199407024531773</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="101">
       <c r="A101">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B101">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="102">
       <c r="A102">
-        <v>0.6199424779454223</v>
+        <v>0.7031997836794691</v>
       </c>
       <c r="B102">
-        <v>0.3800575220545777</v>
+        <v>0.2968002163205309</v>
       </c>
     </row>
     <row r="103">
       <c r="A103">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B103">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="104">
       <c r="A104">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B104">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="105">
       <c r="A105">
-        <v>0.5498452523359121</v>
+        <v>0.6420799356935972</v>
       </c>
       <c r="B105">
-        <v>0.4501547476640879</v>
+        <v>0.3579200643064028</v>
       </c>
     </row>
     <row r="106">
       <c r="A106">
-        <v>0.4917517676904533</v>
+        <v>0.6420799356935972</v>
       </c>
       <c r="B106">
-        <v>0.5082482323095467</v>
+        <v>0.3579200643064028</v>
       </c>
     </row>
     <row r="107">
       <c r="A107">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B107">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="108">
       <c r="A108">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B108">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="109">
       <c r="A109">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B109">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="110">
       <c r="A110">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B110">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="111">
       <c r="A111">
-        <v>0.6537986360375384</v>
+        <v>0.6661742215619185</v>
       </c>
       <c r="B111">
-        <v>0.3462013639624616</v>
+        <v>0.3338257784380815</v>
       </c>
     </row>
     <row r="112">
       <c r="A112">
-        <v>0.8003118571500073</v>
+        <v>0.8380566359458733</v>
       </c>
       <c r="B112">
-        <v>0.1996881428499927</v>
+        <v>0.1619433640541267</v>
       </c>
     </row>
     <row r="113">
       <c r="A113">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B113">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
     <row r="114">
       <c r="A114">
-        <v>0.7930227321826114</v>
+        <v>0.824948703925055</v>
       </c>
       <c r="B114">
-        <v>0.2069772678173886</v>
+        <v>0.175051296074945</v>
       </c>
     </row>
     <row r="115">
       <c r="A115">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B115">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="116">
       <c r="A116">
-        <v>0.7397772836463496</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B116">
-        <v>0.2602227163536504</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="117">
       <c r="A117">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B117">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="118">
       <c r="A118">
-        <v>0.5659720316352707</v>
+        <v>0.6590750771611322</v>
       </c>
       <c r="B118">
-        <v>0.4340279683647293</v>
+        <v>0.3409249228388678</v>
       </c>
     </row>
     <row r="119">
       <c r="A119">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B119">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="120">
       <c r="A120">
-        <v>0.7397772836463496</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B120">
-        <v>0.2602227163536504</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="121">
       <c r="A121">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B121">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="122">
       <c r="A122">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B122">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="123">
       <c r="A123">
-        <v>0.6532384677162565</v>
+        <v>0.5960669561043807</v>
       </c>
       <c r="B123">
-        <v>0.3467615322837435</v>
+        <v>0.4039330438956193</v>
       </c>
     </row>
     <row r="124">
       <c r="A124">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B124">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="125">
       <c r="A125">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B125">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="126">
       <c r="A126">
-        <v>0.8994915014777216</v>
+        <v>0.8749414277318412</v>
       </c>
       <c r="B126">
-        <v>0.1005084985222784</v>
+        <v>0.1250585722681588</v>
       </c>
     </row>
     <row r="127">
       <c r="A127">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B127">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="128">
       <c r="A128">
-        <v>0.8749414277318412</v>
+        <v>0.8994915014777216</v>
       </c>
       <c r="B128">
-        <v>0.1250585722681588</v>
+        <v>0.1005084985222784</v>
       </c>
     </row>
     <row r="129">
       <c r="A129">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B129">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="130">
       <c r="A130">
-        <v>0.7820840370477621</v>
+        <v>0.8466431206713463</v>
       </c>
       <c r="B130">
-        <v>0.2179159629522379</v>
+        <v>0.1533568793286537</v>
       </c>
     </row>
     <row r="131">
       <c r="A131">
-        <v>0.8238111218781662</v>
+        <v>0.8380566359458733</v>
       </c>
       <c r="B131">
-        <v>0.1761888781218338</v>
+        <v>0.1619433640541267</v>
       </c>
     </row>
     <row r="132">
       <c r="A132">
-        <v>0.850880607636742</v>
+        <v>0.863300632083034</v>
       </c>
       <c r="B132">
-        <v>0.149119392363258</v>
+        <v>0.136699367916966</v>
       </c>
     </row>
     <row r="133">
       <c r="A133">
-        <v>0.7441171837957787</v>
+        <v>0.7042392952545217</v>
       </c>
       <c r="B133">
-        <v>0.2558828162042213</v>
+        <v>0.2957607047454783</v>
       </c>
     </row>
     <row r="134">
       <c r="A134">
-        <v>0.8579027536809138</v>
+        <v>0.8003118571500073</v>
       </c>
       <c r="B134">
-        <v>0.1420972463190862</v>
+        <v>0.1996881428499927</v>
       </c>
     </row>
     <row r="135">
       <c r="A135">
-        <v>0.8560506741599387</v>
+        <v>0.7602848156868673</v>
       </c>
       <c r="B135">
-        <v>0.1439493258400613</v>
+        <v>0.2397151843131327</v>
       </c>
     </row>
     <row r="136">
       <c r="A136">
-        <v>0.8466431206713463</v>
+        <v>0.7820840370477621</v>
       </c>
       <c r="B136">
-        <v>0.1533568793286537</v>
+        <v>0.2179159629522379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>